<commit_message>
added guild specific habitat targets
</commit_message>
<xml_diff>
--- a/MP Workbook LAUNCHPAD.xlsx
+++ b/MP Workbook LAUNCHPAD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="360" windowWidth="14430" windowHeight="11355" activeTab="3"/>
+    <workbookView xWindow="1995" yWindow="360" windowWidth="14430" windowHeight="11355" tabRatio="779" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="311">
   <si>
     <t>Scenario</t>
   </si>
@@ -710,15 +710,6 @@
     <t>T30-1 should not be changed (remain Breeding Waterfowl and Meadow)</t>
   </si>
   <si>
-    <t>All DCAs under Gravel in Step 0 should reamin as Gravel (Corridor 1, Phase 8, T1A-3, T35-1, T35-2, T15, T22, T20, T32-2, T35-3, T37-1a, T10-3a, T21-1, T21-2)</t>
-  </si>
-  <si>
-    <t>All DCAs under Brine in Step 0 should reamin as Brine (T10-3W, T2-5, T29-4, T36-3 Addition, T36-3E, T36-3W, T5-4, T8W)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other waterless stay waterless (any Tillage, Till-Brine or Sand Fences in Step 0) (T1A-1 (sand fences), T12-1, T2-3, T2-4, T24 Addition, T3NE, T3SE, T3SW (Tillage), </t>
-  </si>
-  <si>
     <t>Managed Vegetation (2008)</t>
   </si>
   <si>
@@ -824,42 +815,6 @@
     <t>T10-1a waterless only</t>
   </si>
   <si>
-    <t>T13-1 Addition should be sprinklers</t>
-  </si>
-  <si>
-    <t>T23-5 should not be gravel</t>
-  </si>
-  <si>
-    <t>T11 should be Brine</t>
-  </si>
-  <si>
-    <t>T23NE should be brine</t>
-  </si>
-  <si>
-    <t>T23SE should be sand fences</t>
-  </si>
-  <si>
-    <t>T25-3 cannot be tillage or gravel</t>
-  </si>
-  <si>
-    <t>T26 no tilalge, sand fences or brine</t>
-  </si>
-  <si>
-    <t>T27 Addtion only Brine</t>
-  </si>
-  <si>
-    <t>T32-1 should stay as Meadow</t>
-  </si>
-  <si>
-    <t>T29-3 only Brine</t>
-  </si>
-  <si>
-    <t>T13-1 Additiom waterless only</t>
-  </si>
-  <si>
-    <t>T16 statys MWF and MSB</t>
-  </si>
-  <si>
     <t>T3SE, T4-3, T4-3 Addition no ponds</t>
   </si>
   <si>
@@ -914,12 +869,6 @@
     <t>Sand Fences Area Limit (lakewide total)</t>
   </si>
   <si>
-    <t>decimal % of Base Acreage</t>
-  </si>
-  <si>
-    <t>Habitat Acreage Target (each guild)</t>
-  </si>
-  <si>
     <t>Transition Type</t>
   </si>
   <si>
@@ -966,6 +915,54 @@
   </si>
   <si>
     <t>T1A-2 to stay as BWF</t>
+  </si>
+  <si>
+    <t>T16 stays MWF and MSB</t>
+  </si>
+  <si>
+    <t>Habitat Area Targets</t>
+  </si>
+  <si>
+    <t>decimal % of Base case area</t>
+  </si>
+  <si>
+    <t>All DCAs under waterless DCM (Tillage, Brine, Gravel, Sand Fences) in Step 0 should be kept as-is.</t>
+  </si>
+  <si>
+    <t>T13-1 Addition sprinklers only</t>
+  </si>
+  <si>
+    <t>T23-5 should no gravel</t>
+  </si>
+  <si>
+    <t>T11 should Brine only</t>
+  </si>
+  <si>
+    <t>T23NE Brine only</t>
+  </si>
+  <si>
+    <t>T23SE no Tillage</t>
+  </si>
+  <si>
+    <t>T25-3 no Tillage or Gravel</t>
+  </si>
+  <si>
+    <t>T26 should no tillage, sand fences or brine</t>
+  </si>
+  <si>
+    <t>T27 Addtion Brine only</t>
+  </si>
+  <si>
+    <t>T29-3 Brine only</t>
+  </si>
+  <si>
+    <t>All Meadow stays as-is</t>
+  </si>
+  <si>
+    <t>T13-1 Addition waterless only</t>
+  </si>
+  <si>
+    <t>Note: in general case, waterless DCMs have no habitat value. In a few specific instances in Base case, some DCAs under waterless DCMs had habitat (see "Custom HV and WD" sheet).</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1389,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1609,6 +1606,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -2049,8 +2052,8 @@
   </sheetPr>
   <dimension ref="A1:CP200"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2066,7 @@
     <col min="8" max="8" width="16.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="62" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" style="62" customWidth="1"/>
-    <col min="11" max="11" width="37" style="62" customWidth="1"/>
+    <col min="11" max="11" width="35" style="62" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" style="62" customWidth="1"/>
     <col min="13" max="13" width="14.140625" style="62" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" style="62" customWidth="1"/>
@@ -2126,19 +2129,26 @@
         <v>5</v>
       </c>
       <c r="G2" s="60" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="H2" s="60" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="I2" s="60" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="K2" s="100" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="L2" s="101"/>
       <c r="M2" s="66"/>
+      <c r="O2" s="100" t="s">
+        <v>296</v>
+      </c>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="109" t="s">
+        <v>297</v>
+      </c>
       <c r="AI2" s="63"/>
       <c r="AJ2" s="62"/>
       <c r="AW2" s="63"/>
@@ -2154,7 +2164,7 @@
       <c r="CO2" s="62"/>
       <c r="CP2" s="62"/>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2189,14 +2199,21 @@
         <v>7</v>
       </c>
       <c r="K3" s="86" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="L3" s="87">
         <v>3</v>
       </c>
       <c r="M3" s="62" t="s">
-        <v>283</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="O3" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="87">
+        <v>0.9</v>
+      </c>
+      <c r="Q3" s="110"/>
       <c r="AI3" s="63"/>
       <c r="AJ3" s="62"/>
       <c r="AW3" s="63"/>
@@ -2247,14 +2264,21 @@
         <v>7</v>
       </c>
       <c r="K4" s="86" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="L4" s="87">
         <v>3</v>
       </c>
       <c r="M4" s="62" t="s">
-        <v>283</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="O4" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="87">
+        <v>0.9</v>
+      </c>
+      <c r="Q4" s="110"/>
       <c r="AI4" s="63"/>
       <c r="AJ4" s="62"/>
       <c r="AW4" s="63"/>
@@ -2307,14 +2331,21 @@
         <v>0</v>
       </c>
       <c r="K5" s="86" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="L5" s="87">
-        <v>0.9</v>
+        <v>100</v>
       </c>
       <c r="M5" s="62" t="s">
-        <v>294</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="O5" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="110"/>
       <c r="AI5" s="63"/>
       <c r="AJ5" s="62"/>
       <c r="AW5" s="63"/>
@@ -2367,14 +2398,21 @@
         <v>0</v>
       </c>
       <c r="K6" s="86" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="L6" s="87">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M6" s="62" t="s">
-        <v>283</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="O6" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="87">
+        <v>0.9</v>
+      </c>
+      <c r="Q6" s="110"/>
       <c r="AI6" s="63"/>
       <c r="AJ6" s="62"/>
       <c r="AW6" s="63"/>
@@ -2426,14 +2464,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K7" s="86" t="s">
-        <v>293</v>
-      </c>
-      <c r="L7" s="87">
-        <v>100</v>
-      </c>
-      <c r="M7" s="62" t="s">
-        <v>283</v>
+      <c r="O7" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="87">
+        <v>0.9</v>
       </c>
       <c r="AI7" s="63"/>
       <c r="AJ7" s="62"/>
@@ -2600,13 +2635,13 @@
         <v>9</v>
       </c>
       <c r="H11" s="58" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="K11" s="53" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="M11" s="98" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="N11" s="99"/>
       <c r="O11" s="66" t="s">
@@ -2663,13 +2698,13 @@
         <v>38</v>
       </c>
       <c r="M12" s="97" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N12" s="41" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="O12" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="AI12" s="63"/>
       <c r="AJ12" s="62"/>
@@ -2722,13 +2757,13 @@
         <v>63</v>
       </c>
       <c r="M13" s="97" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="N13" s="41" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="O13" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="AI13" s="63"/>
       <c r="AJ13" s="62"/>
@@ -2781,13 +2816,13 @@
         <v>34</v>
       </c>
       <c r="M14" s="97" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="O14" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="AI14" s="63"/>
       <c r="AJ14" s="62"/>
@@ -2843,10 +2878,10 @@
         <v>63</v>
       </c>
       <c r="N15" s="41" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="O15" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="AI15" s="63"/>
       <c r="AJ15" s="62"/>
@@ -2902,10 +2937,10 @@
         <v>58</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="O16" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="AI16" s="63"/>
       <c r="AJ16" s="62"/>
@@ -3097,7 +3132,7 @@
         <v>15</v>
       </c>
       <c r="I21" s="93" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="J21"/>
       <c r="K21" s="57"/>
@@ -3187,7 +3222,7 @@
       </c>
       <c r="J22"/>
       <c r="K22" s="94" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="L22" s="94"/>
       <c r="M22" s="94"/>
@@ -3301,7 +3336,7 @@
       </c>
       <c r="J23"/>
       <c r="K23" s="95" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="L23" s="78"/>
       <c r="M23" s="78"/>
@@ -3415,7 +3450,7 @@
       </c>
       <c r="J24"/>
       <c r="K24" s="96" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="L24" s="79"/>
       <c r="M24" s="79"/>
@@ -21434,9 +21469,10 @@
       <c r="J200" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21458,7 +21494,7 @@
           <x14:formula1>
             <xm:f>'Generic HV &amp; WD'!$A$28:$A$32</xm:f>
           </x14:formula1>
-          <xm:sqref>M16 M12:M15</xm:sqref>
+          <xm:sqref>M12:M16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -21474,7 +21510,7 @@
   <dimension ref="A1:W248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C249" sqref="C249"/>
     </sheetView>
   </sheetViews>
@@ -21533,7 +21569,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D2" s="1">
         <v>0.1619548872180451</v>
@@ -21570,7 +21606,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D3" s="1">
         <v>0.24035532994923858</v>
@@ -21606,7 +21642,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -21642,7 +21678,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -21678,7 +21714,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -21714,7 +21750,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -21750,7 +21786,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -21786,7 +21822,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -21822,7 +21858,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -21858,7 +21894,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -21894,7 +21930,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -21930,7 +21966,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -21961,7 +21997,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -21992,7 +22028,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -22023,7 +22059,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -22054,7 +22090,7 @@
         <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -22085,7 +22121,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -22116,7 +22152,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -22147,7 +22183,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -22178,7 +22214,7 @@
         <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -22209,7 +22245,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -22240,7 +22276,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -22271,7 +22307,7 @@
         <v>29</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -22302,7 +22338,7 @@
         <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -22333,7 +22369,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -22364,7 +22400,7 @@
         <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -22395,7 +22431,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -22426,7 +22462,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -22457,7 +22493,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -22488,7 +22524,7 @@
         <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -22519,7 +22555,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -22550,7 +22586,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -22581,7 +22617,7 @@
         <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -22612,7 +22648,7 @@
         <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -22643,7 +22679,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -22674,7 +22710,7 @@
         <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -22705,7 +22741,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -22736,7 +22772,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D39" s="1">
         <v>0.17260904187551165</v>
@@ -22767,7 +22803,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D40" s="1">
         <v>0.14497210174440919</v>
@@ -22798,7 +22834,7 @@
         <v>29</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -22829,7 +22865,7 @@
         <v>36</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -22860,7 +22896,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -22891,7 +22927,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -22922,7 +22958,7 @@
         <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -22953,7 +22989,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -22984,7 +23020,7 @@
         <v>36</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -23015,7 +23051,7 @@
         <v>36</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -23046,7 +23082,7 @@
         <v>36</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -23077,7 +23113,7 @@
         <v>36</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -23108,7 +23144,7 @@
         <v>36</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -23139,7 +23175,7 @@
         <v>36</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
@@ -23170,7 +23206,7 @@
         <v>36</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -23201,7 +23237,7 @@
         <v>38</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -23232,7 +23268,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -23263,7 +23299,7 @@
         <v>36</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -23294,7 +23330,7 @@
         <v>36</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -23325,7 +23361,7 @@
         <v>36</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -23356,7 +23392,7 @@
         <v>36</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -23387,7 +23423,7 @@
         <v>36</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -23418,7 +23454,7 @@
         <v>36</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
@@ -23449,7 +23485,7 @@
         <v>36</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D62" s="1">
         <v>0.16832229580573951</v>
@@ -23480,7 +23516,7 @@
         <v>36</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D63" s="1">
         <v>0.16576666666666665</v>
@@ -23511,7 +23547,7 @@
         <v>29</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
@@ -23542,7 +23578,7 @@
         <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D65" s="1">
         <v>0</v>
@@ -23573,7 +23609,7 @@
         <v>29</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
@@ -23604,7 +23640,7 @@
         <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
@@ -23639,7 +23675,7 @@
         <v>36</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D68" s="1">
         <v>0.34571304221674165</v>
@@ -23670,7 +23706,7 @@
         <v>29</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D69" s="1">
         <v>0</v>
@@ -23701,7 +23737,7 @@
         <v>29</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
@@ -23732,7 +23768,7 @@
         <v>43</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D71" s="1">
         <v>5.7664884135472369E-2</v>
@@ -23763,7 +23799,7 @@
         <v>43</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D72" s="1">
         <v>2.9393043531919214E-2</v>
@@ -23794,7 +23830,7 @@
         <v>29</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -23825,7 +23861,7 @@
         <v>29</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -23856,7 +23892,7 @@
         <v>43</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -23887,7 +23923,7 @@
         <v>36</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D76" s="1">
         <v>0.34112343966712899</v>
@@ -23918,7 +23954,7 @@
         <v>36</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
@@ -23949,7 +23985,7 @@
         <v>29</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -23980,7 +24016,7 @@
         <v>29</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -24011,7 +24047,7 @@
         <v>38</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D80" s="1">
         <v>0</v>
@@ -24042,7 +24078,7 @@
         <v>38</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -24073,7 +24109,7 @@
         <v>38</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -24104,7 +24140,7 @@
         <v>43</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D83" s="1">
         <v>6.7301038062283741E-2</v>
@@ -24135,7 +24171,7 @@
         <v>43</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -24166,7 +24202,7 @@
         <v>43</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D85" s="1">
         <v>2.9418934495912277E-2</v>
@@ -24197,7 +24233,7 @@
         <v>43</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -24228,7 +24264,7 @@
         <v>43</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
@@ -24259,7 +24295,7 @@
         <v>43</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D88" s="1">
         <v>0</v>
@@ -24290,7 +24326,7 @@
         <v>36</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D89" s="1">
         <v>0</v>
@@ -24321,7 +24357,7 @@
         <v>36</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
@@ -24352,7 +24388,7 @@
         <v>36</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -24383,7 +24419,7 @@
         <v>36</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
@@ -24414,7 +24450,7 @@
         <v>36</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -24445,7 +24481,7 @@
         <v>36</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D94" s="1">
         <v>0</v>
@@ -24476,7 +24512,7 @@
         <v>29</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -24507,7 +24543,7 @@
         <v>29</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
@@ -24538,7 +24574,7 @@
         <v>36</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D97" s="1">
         <v>0.33217592592592587</v>
@@ -24569,7 +24605,7 @@
         <v>124</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
@@ -24600,7 +24636,7 @@
         <v>36</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D99" s="1">
         <v>0</v>
@@ -24631,7 +24667,7 @@
         <v>36</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D100" s="1">
         <v>0.36257183908045981</v>
@@ -24662,7 +24698,7 @@
         <v>29</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D101" s="1">
         <v>0.3681141439205956</v>
@@ -24693,7 +24729,7 @@
         <v>129</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D102" s="1">
         <v>0.16350000000000001</v>
@@ -24724,7 +24760,7 @@
         <v>129</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D103" s="1">
         <v>0.20609137055837562</v>
@@ -24755,7 +24791,7 @@
         <v>29</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D104" s="1">
         <v>0</v>
@@ -24786,7 +24822,7 @@
         <v>129</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D105" s="1">
         <v>0.16350000000000001</v>
@@ -24817,7 +24853,7 @@
         <v>129</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D106" s="1">
         <v>0.16350000000000001</v>
@@ -24848,7 +24884,7 @@
         <v>129</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D107" s="1">
         <v>0.16350000000000001</v>
@@ -24879,7 +24915,7 @@
         <v>129</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D108" s="1">
         <v>0.16350000000000001</v>
@@ -24910,7 +24946,7 @@
         <v>129</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D109" s="1">
         <v>0.22174999999999997</v>
@@ -24941,7 +24977,7 @@
         <v>129</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D110" s="1">
         <v>0.16350000000000001</v>
@@ -24972,7 +25008,7 @@
         <v>129</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D111" s="1">
         <v>0.16350000000000001</v>
@@ -25003,7 +25039,7 @@
         <v>129</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D112" s="1">
         <v>0.16350000000000001</v>
@@ -25034,7 +25070,7 @@
         <v>129</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D113" s="1">
         <v>0.16350000000000001</v>
@@ -25065,7 +25101,7 @@
         <v>129</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D114" s="1">
         <v>0.16350000000000001</v>
@@ -25096,7 +25132,7 @@
         <v>129</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D115" s="1">
         <v>0.16350000000000001</v>
@@ -25127,7 +25163,7 @@
         <v>129</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D116" s="1">
         <v>0.16350000000000001</v>
@@ -25158,7 +25194,7 @@
         <v>129</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D117" s="1">
         <v>0.16350000000000001</v>
@@ -25189,7 +25225,7 @@
         <v>129</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D118" s="1">
         <v>0.16350000000000001</v>
@@ -25220,7 +25256,7 @@
         <v>129</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D119" s="1">
         <v>0.16350000000000001</v>
@@ -25251,7 +25287,7 @@
         <v>129</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D120" s="1">
         <v>0.16350000000000001</v>
@@ -25282,7 +25318,7 @@
         <v>129</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D121" s="1">
         <v>0.16350000000000001</v>
@@ -25313,7 +25349,7 @@
         <v>129</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D122" s="1">
         <v>0.16350000000000001</v>
@@ -25344,7 +25380,7 @@
         <v>129</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D123" s="1">
         <v>0.16350000000000001</v>
@@ -25375,7 +25411,7 @@
         <v>129</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D124" s="1">
         <v>0.16350000000000001</v>
@@ -25406,7 +25442,7 @@
         <v>129</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D125" s="1">
         <v>0.16350000000000001</v>
@@ -25437,7 +25473,7 @@
         <v>129</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D126" s="1">
         <v>0.16350000000000001</v>
@@ -25468,7 +25504,7 @@
         <v>129</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D127" s="1">
         <v>0.16350000000000001</v>
@@ -25499,7 +25535,7 @@
         <v>129</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D128" s="1">
         <v>0.22174999999999997</v>
@@ -25530,7 +25566,7 @@
         <v>129</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D129" s="1">
         <v>0.22174999999999997</v>
@@ -25561,7 +25597,7 @@
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D130" s="1">
         <v>0.22174999999999997</v>
@@ -25592,7 +25628,7 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D131" s="1">
         <v>0.16350000000000001</v>
@@ -25623,7 +25659,7 @@
         <v>129</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D132" s="1">
         <v>0.16350000000000001</v>
@@ -25654,7 +25690,7 @@
         <v>129</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D133" s="1">
         <v>0.16350000000000001</v>
@@ -25685,7 +25721,7 @@
         <v>129</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D134" s="1">
         <v>0.16350000000000001</v>
@@ -25716,7 +25752,7 @@
         <v>129</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D135" s="1">
         <v>0.16350000000000001</v>
@@ -25747,7 +25783,7 @@
         <v>129</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D136" s="1">
         <v>0.16350000000000001</v>
@@ -25778,7 +25814,7 @@
         <v>129</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D137" s="1">
         <v>0.16350000000000001</v>
@@ -25809,7 +25845,7 @@
         <v>129</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D138" s="1">
         <v>0.16350000000000001</v>
@@ -25840,7 +25876,7 @@
         <v>129</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D139" s="1">
         <v>0.16350000000000001</v>
@@ -25871,7 +25907,7 @@
         <v>129</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D140" s="1">
         <v>0.16350000000000001</v>
@@ -25902,7 +25938,7 @@
         <v>129</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D141" s="1">
         <v>0.16350000000000001</v>
@@ -25933,7 +25969,7 @@
         <v>129</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D142" s="1">
         <v>0.16350000000000001</v>
@@ -25964,7 +26000,7 @@
         <v>129</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D143" s="1">
         <v>0.16350000000000001</v>
@@ -25995,7 +26031,7 @@
         <v>129</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D144" s="1">
         <v>0.16340852130325814</v>
@@ -26026,7 +26062,7 @@
         <v>129</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D145" s="1">
         <v>0.16350000000000001</v>
@@ -26057,7 +26093,7 @@
         <v>129</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D146" s="1">
         <v>0.16350000000000001</v>
@@ -26088,7 +26124,7 @@
         <v>129</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D147" s="1">
         <v>0.16347607052896726</v>
@@ -26119,7 +26155,7 @@
         <v>129</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D148" s="1">
         <v>0.16350000000000001</v>
@@ -26150,7 +26186,7 @@
         <v>129</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D149" s="1">
         <v>0.16350000000000001</v>
@@ -26181,7 +26217,7 @@
         <v>129</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D150" s="1">
         <v>0.16350000000000001</v>
@@ -26212,7 +26248,7 @@
         <v>129</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D151" s="1">
         <v>0.16336633663366337</v>
@@ -26243,7 +26279,7 @@
         <v>129</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D152" s="1">
         <v>0.16347607052896726</v>
@@ -26274,7 +26310,7 @@
         <v>129</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D153" s="1">
         <v>0.16350000000000001</v>
@@ -26305,7 +26341,7 @@
         <v>129</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D154" s="1">
         <v>0.16350000000000001</v>
@@ -26336,7 +26372,7 @@
         <v>129</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D155" s="1">
         <v>0.16350000000000001</v>
@@ -26367,7 +26403,7 @@
         <v>129</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D156" s="1">
         <v>0.16350000000000001</v>
@@ -26398,7 +26434,7 @@
         <v>129</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D157" s="1">
         <v>0.16350000000000001</v>
@@ -26429,7 +26465,7 @@
         <v>129</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D158" s="1">
         <v>0.16337349397590362</v>
@@ -26460,7 +26496,7 @@
         <v>129</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D159" s="1">
         <v>0.16348837209302325</v>
@@ -26491,7 +26527,7 @@
         <v>38</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D160" s="1">
         <v>0</v>
@@ -26522,7 +26558,7 @@
         <v>29</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D161" s="1">
         <v>0</v>
@@ -26553,7 +26589,7 @@
         <v>30</v>
       </c>
       <c r="C162" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D162" s="22">
         <v>0</v>
@@ -26593,7 +26629,7 @@
         <v>33</v>
       </c>
       <c r="C163" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D163" s="22">
         <v>0</v>
@@ -26631,7 +26667,7 @@
         <v>33</v>
       </c>
       <c r="C164" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D164" s="22">
         <v>0</v>
@@ -26669,7 +26705,7 @@
         <v>33</v>
       </c>
       <c r="C165" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D165" s="22">
         <v>0</v>
@@ -26707,7 +26743,7 @@
         <v>38</v>
       </c>
       <c r="C166" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D166" s="22">
         <v>0</v>
@@ -26745,7 +26781,7 @@
         <v>30</v>
       </c>
       <c r="C167" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D167" s="22">
         <v>0</v>
@@ -26783,7 +26819,7 @@
         <v>33</v>
       </c>
       <c r="C168" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D168" s="22">
         <v>0</v>
@@ -26821,7 +26857,7 @@
         <v>36</v>
       </c>
       <c r="C169" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D169" s="22">
         <v>0</v>
@@ -26859,7 +26895,7 @@
         <v>36</v>
       </c>
       <c r="C170" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D170" s="22">
         <v>0</v>
@@ -26897,7 +26933,7 @@
         <v>33</v>
       </c>
       <c r="C171" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D171" s="22">
         <v>0</v>
@@ -26935,7 +26971,7 @@
         <v>54</v>
       </c>
       <c r="C172" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D172" s="22">
         <v>0</v>
@@ -26973,7 +27009,7 @@
         <v>54</v>
       </c>
       <c r="C173" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D173" s="22">
         <v>0</v>
@@ -27011,7 +27047,7 @@
         <v>33</v>
       </c>
       <c r="C174" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D174" s="22">
         <v>0</v>
@@ -27049,7 +27085,7 @@
         <v>33</v>
       </c>
       <c r="C175" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D175" s="22">
         <v>0</v>
@@ -27087,7 +27123,7 @@
         <v>29</v>
       </c>
       <c r="C176" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D176" s="22">
         <v>0</v>
@@ -27125,7 +27161,7 @@
         <v>33</v>
       </c>
       <c r="C177" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D177" s="22">
         <v>0</v>
@@ -27158,7 +27194,7 @@
         <v>36</v>
       </c>
       <c r="C178" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D178" s="22">
         <v>0</v>
@@ -27191,7 +27227,7 @@
         <v>36</v>
       </c>
       <c r="C179" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D179" s="22">
         <v>0</v>
@@ -27224,7 +27260,7 @@
         <v>29</v>
       </c>
       <c r="C180" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D180" s="22">
         <v>0</v>
@@ -27257,7 +27293,7 @@
         <v>29</v>
       </c>
       <c r="C181" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D181" s="22">
         <v>0</v>
@@ -27290,7 +27326,7 @@
         <v>29</v>
       </c>
       <c r="C182" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D182" s="22">
         <v>0</v>
@@ -27323,7 +27359,7 @@
         <v>29</v>
       </c>
       <c r="C183" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D183" s="22">
         <v>0</v>
@@ -27356,7 +27392,7 @@
         <v>43</v>
       </c>
       <c r="C184" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D184" s="22">
         <v>0</v>
@@ -27389,7 +27425,7 @@
         <v>36</v>
       </c>
       <c r="C185" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D185" s="22">
         <v>0.25623790594558404</v>
@@ -27422,7 +27458,7 @@
         <v>29</v>
       </c>
       <c r="C186" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D186" s="22">
         <v>0.3072719469000792</v>
@@ -27455,7 +27491,7 @@
         <v>30</v>
       </c>
       <c r="C187" s="22" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D187" s="22">
         <v>0</v>
@@ -27488,7 +27524,7 @@
         <v>30</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D188" s="1">
         <v>0</v>
@@ -27521,7 +27557,7 @@
         <v>26</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D189" s="1">
         <v>0</v>
@@ -27554,7 +27590,7 @@
         <v>34</v>
       </c>
       <c r="C190" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D190" s="1">
         <v>0</v>
@@ -27587,7 +27623,7 @@
         <v>26</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D191" s="1">
         <v>0</v>
@@ -27620,7 +27656,7 @@
         <v>199</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D192" s="1">
         <v>0.61348618826838841</v>
@@ -27653,7 +27689,7 @@
         <v>26</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D193" s="1">
         <v>0</v>
@@ -27686,7 +27722,7 @@
         <v>36</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D194" s="1">
         <v>0</v>
@@ -27719,7 +27755,7 @@
         <v>26</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D195" s="1">
         <v>0</v>
@@ -27752,7 +27788,7 @@
         <v>26</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D196" s="1">
         <v>0</v>
@@ -27785,7 +27821,7 @@
         <v>26</v>
       </c>
       <c r="C197" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D197" s="1">
         <v>0</v>
@@ -27818,7 +27854,7 @@
         <v>124</v>
       </c>
       <c r="C198" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D198" s="1">
         <v>0.22579427120177961</v>
@@ -27851,7 +27887,7 @@
         <v>124</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D199" s="1">
         <v>0.27712907665452824</v>
@@ -27884,7 +27920,7 @@
         <v>26</v>
       </c>
       <c r="C200" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D200" s="1">
         <v>0</v>
@@ -27917,7 +27953,7 @@
         <v>34</v>
       </c>
       <c r="C201" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D201" s="1">
         <v>0</v>
@@ -27950,7 +27986,7 @@
         <v>34</v>
       </c>
       <c r="C202" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D202" s="1">
         <v>0</v>
@@ -27983,7 +28019,7 @@
         <v>34</v>
       </c>
       <c r="C203" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D203" s="1">
         <v>0</v>
@@ -28016,7 +28052,7 @@
         <v>5</v>
       </c>
       <c r="C204" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D204" s="1">
         <v>0.5938570581787751</v>
@@ -28049,7 +28085,7 @@
         <v>5</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D205" s="1">
         <v>0.4280920212459568</v>
@@ -28082,7 +28118,7 @@
         <v>38</v>
       </c>
       <c r="C206" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D206" s="1">
         <v>0</v>
@@ -28115,7 +28151,7 @@
         <v>124</v>
       </c>
       <c r="C207" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D207" s="1">
         <v>0.70311614561032765</v>
@@ -28148,7 +28184,7 @@
         <v>26</v>
       </c>
       <c r="C208" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D208" s="1">
         <v>2.939815783088038E-2</v>
@@ -28181,7 +28217,7 @@
         <v>26</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D209" s="1">
         <v>0</v>
@@ -28214,7 +28250,7 @@
         <v>26</v>
       </c>
       <c r="C210" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D210" s="1">
         <v>0</v>
@@ -28247,7 +28283,7 @@
         <v>26</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D211" s="1">
         <v>0</v>
@@ -28280,7 +28316,7 @@
         <v>5</v>
       </c>
       <c r="C212" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D212" s="1">
         <v>0.57999672167082694</v>
@@ -28313,7 +28349,7 @@
         <v>5</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D213" s="1">
         <v>0.53473837997478868</v>
@@ -28346,7 +28382,7 @@
         <v>26</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D214" s="1">
         <v>6.7304979947679047E-2</v>
@@ -28379,7 +28415,7 @@
         <v>68</v>
       </c>
       <c r="C215" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D215" s="1">
         <v>0</v>
@@ -28412,7 +28448,7 @@
         <v>33</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D216" s="1">
         <v>0</v>
@@ -28445,7 +28481,7 @@
         <v>33</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D217" s="1">
         <v>0</v>
@@ -28478,7 +28514,7 @@
         <v>33</v>
       </c>
       <c r="C218" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D218" s="1">
         <v>0</v>
@@ -28511,7 +28547,7 @@
         <v>33</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D219" s="1">
         <v>0</v>
@@ -28544,7 +28580,7 @@
         <v>34</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D220" s="1">
         <v>0</v>
@@ -28577,7 +28613,7 @@
         <v>34</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D221" s="1">
         <v>0</v>
@@ -28610,7 +28646,7 @@
         <v>34</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D222" s="1">
         <v>0</v>
@@ -28643,7 +28679,7 @@
         <v>34</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D223" s="1">
         <v>0</v>
@@ -28676,7 +28712,7 @@
         <v>38</v>
       </c>
       <c r="C224" s="13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D224" s="1">
         <v>0</v>
@@ -28709,7 +28745,7 @@
         <v>1</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D225" s="20" t="e">
         <f>NA()</f>
@@ -28748,7 +28784,7 @@
         <v>2</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D226" s="20" t="e">
         <f>NA()</f>
@@ -28775,7 +28811,7 @@
         <v>1.4672727272727271</v>
       </c>
       <c r="J226" s="51" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="W226" s="1"/>
     </row>
@@ -28787,7 +28823,7 @@
         <v>45</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D227" s="20" t="e">
         <f>NA()</f>
@@ -28814,7 +28850,7 @@
         <v>1.4672727272727271</v>
       </c>
       <c r="J227" s="51" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="W227" s="1"/>
     </row>
@@ -28826,7 +28862,7 @@
         <v>82</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D228" s="20" t="e">
         <f>NA()</f>
@@ -28853,7 +28889,7 @@
         <v>1.4672727272727271</v>
       </c>
       <c r="J228" s="51" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K228" s="19">
         <f>300/1100</f>
@@ -28869,7 +28905,7 @@
         <v>4</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D229" s="20" t="e">
         <f>NA()</f>
@@ -28905,7 +28941,7 @@
         <v>49</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D230" s="20" t="e">
         <f>NA()</f>
@@ -28941,7 +28977,7 @@
         <v>31</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D231" s="20" t="e">
         <f>NA()</f>
@@ -28977,7 +29013,7 @@
         <v>65</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D232" s="20" t="e">
         <f>NA()</f>
@@ -29013,7 +29049,7 @@
         <v>79</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D233" s="20" t="e">
         <f>NA()</f>
@@ -29049,7 +29085,7 @@
         <v>55</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D234" s="20" t="e">
         <f>NA()</f>
@@ -29085,7 +29121,7 @@
         <v>210</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D235" s="20" t="e">
         <f>NA()</f>
@@ -29121,7 +29157,7 @@
         <v>100</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D236" s="20" t="e">
         <f>NA()</f>
@@ -29157,7 +29193,7 @@
         <v>1</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D237" s="20" t="e">
         <f>NA()</f>
@@ -29206,7 +29242,7 @@
         <v>2</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D238" s="20" t="e">
         <f>NA()</f>
@@ -29241,7 +29277,7 @@
         <v>45</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D239" s="20" t="e">
         <f>NA()</f>
@@ -29276,7 +29312,7 @@
         <v>82</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D240" s="20" t="e">
         <f>NA()</f>
@@ -29311,7 +29347,7 @@
         <v>4</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D241" s="20" t="e">
         <f>NA()</f>
@@ -29346,7 +29382,7 @@
         <v>49</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D242" s="20" t="e">
         <f>NA()</f>
@@ -29381,7 +29417,7 @@
         <v>31</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D243" s="20" t="e">
         <f>NA()</f>
@@ -29416,7 +29452,7 @@
         <v>65</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D244" s="20" t="e">
         <f>NA()</f>
@@ -29451,7 +29487,7 @@
         <v>79</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D245" s="20" t="e">
         <f>NA()</f>
@@ -29486,7 +29522,7 @@
         <v>55</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D246" s="20" t="e">
         <f>NA()</f>
@@ -29521,7 +29557,7 @@
         <v>210</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D247" s="20" t="e">
         <f>NA()</f>
@@ -29556,7 +29592,7 @@
         <v>100</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D248" s="20" t="e">
         <f>NA()</f>
@@ -29601,8 +29637,8 @@
   </sheetPr>
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29647,7 +29683,7 @@
         <v>215</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>16</v>
@@ -29695,7 +29731,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C4" s="28">
         <f>IFERROR(
@@ -29755,7 +29791,7 @@
         <v>4.3599999999999994</v>
       </c>
       <c r="R4" s="49" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="S4" s="50">
         <v>2.73</v>
@@ -29769,7 +29805,7 @@
         <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C5" s="28">
         <f>IFERROR(
@@ -29829,7 +29865,7 @@
         <v>1.35</v>
       </c>
       <c r="R5" s="49" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="S5" s="50">
         <v>2.68</v>
@@ -29843,7 +29879,7 @@
         <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C6" s="28">
         <f>IFERROR(
@@ -29903,7 +29939,7 @@
         <v>1.49</v>
       </c>
       <c r="R6" s="49" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S6" s="50">
         <v>1.01</v>
@@ -29914,7 +29950,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C7" s="28">
         <f>IFERROR(
@@ -29974,7 +30010,7 @@
         <v>0.72</v>
       </c>
       <c r="R7" s="49" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S7" s="50">
         <v>3.18</v>
@@ -29985,7 +30021,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C8" s="28">
         <f>IFERROR(
@@ -30045,13 +30081,13 @@
         <v>3.5100000000000002</v>
       </c>
       <c r="R8" s="49" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="S8" s="50">
         <v>3.13</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:27" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -30059,7 +30095,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C9" s="28">
         <f>IFERROR(
@@ -30119,7 +30155,7 @@
         <v>0.98</v>
       </c>
       <c r="R9" s="49" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S9" s="50">
         <v>3.86</v>
@@ -30130,7 +30166,7 @@
         <v>199</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C10" s="28">
         <f>IFERROR(
@@ -30190,13 +30226,13 @@
         <v>1.51</v>
       </c>
       <c r="R10" s="49" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="S10" s="50">
         <v>5.38</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:27" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -30204,7 +30240,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C11" s="28">
         <f>IFERROR(
@@ -30269,7 +30305,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C12" s="28">
         <f>IFERROR(
@@ -30334,7 +30370,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C13" s="28">
         <f>IFERROR(
@@ -30399,7 +30435,7 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C14" s="28">
         <f>IFERROR(
@@ -30464,7 +30500,7 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C15" s="28">
         <f>IFERROR(
@@ -30529,7 +30565,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C16" s="28">
         <f>IFERROR(
@@ -30659,7 +30695,7 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C18" s="28">
         <f>IFERROR(
@@ -30724,7 +30760,7 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C19" s="28">
         <f>IFERROR(
@@ -30789,7 +30825,7 @@
         <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C20" s="28">
         <f>IFERROR(
@@ -30854,7 +30890,7 @@
         <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C21" s="28">
         <f>IFERROR(
@@ -30919,7 +30955,7 @@
         <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C22" s="28">
         <f>IFERROR(
@@ -30984,7 +31020,7 @@
         <v>210</v>
       </c>
       <c r="B23" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C23" s="28">
         <f>IFERROR(
@@ -31049,7 +31085,7 @@
         <v>216</v>
       </c>
       <c r="B24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C24" s="28">
         <f>IFERROR(
@@ -31114,7 +31150,7 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C25" s="28">
         <f>IFERROR(
@@ -31179,7 +31215,7 @@
         <v>217</v>
       </c>
       <c r="B26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C26" s="28">
         <f>IFERROR(
@@ -31244,7 +31280,7 @@
         <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C27" s="28">
         <f>IFERROR(
@@ -31319,11 +31355,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!E:E, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A28, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A28, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    K28
-)</f>
-        <v>2.0826061694499486E-2</v>
+        <v>0</v>
       </c>
       <c r="E28" s="28">
         <f>IFERROR(
@@ -31333,17 +31365,9 @@
         <v>0</v>
       </c>
       <c r="F28" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!G:G, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A28, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A28, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    M28
-)</f>
-        <v>5.3022839529496227E-2</v>
+        <v>0</v>
       </c>
       <c r="G28" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!H:H, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A28, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A28, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    N28
-)</f>
         <v>0</v>
       </c>
       <c r="H28" s="30">
@@ -31514,32 +31538,16 @@
         <v>0</v>
       </c>
       <c r="D31" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!E:E, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    K31
-)</f>
-        <v>4.9154589371980681E-2</v>
+        <v>0</v>
       </c>
       <c r="E31" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!F:F, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    L31
-)</f>
-        <v>0.15378421900161032</v>
+        <v>0</v>
       </c>
       <c r="F31" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!G:G, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    M31
-)</f>
-        <v>0.33055555555555555</v>
+        <v>0</v>
       </c>
       <c r="G31" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!H:H, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A31, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    N31
-)</f>
-        <v>1.7230273752012883E-2</v>
+        <v>0</v>
       </c>
       <c r="H31" s="30">
         <v>0</v>
@@ -31586,25 +31594,13 @@
         <v>0</v>
       </c>
       <c r="E32" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!F:F, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A32, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A32, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    L32
-)</f>
-        <v>3.8189448887106923E-2</v>
+        <v>0</v>
       </c>
       <c r="F32" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!G:G, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A32, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A32, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    M32
-)</f>
-        <v>0.14687311131219599</v>
+        <v>0</v>
       </c>
       <c r="G32" s="28">
-        <f>IFERROR(
-    SUMIFS('Custom HV &amp; WD'!H:H, 'Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A32, 'Custom HV &amp; WD'!$C:$C, "Base")/COUNTIFS('Custom HV &amp; WD'!$B:$B, 'Generic HV &amp; WD'!$A32, 'Custom HV &amp; WD'!$C:$C, "Base"),
-    N32
-)</f>
-        <v>2.414330218068536E-3</v>
+        <v>0</v>
       </c>
       <c r="H32" s="30">
         <v>0</v>
@@ -31764,6 +31760,9 @@
     </row>
     <row r="35" spans="1:20" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="R36"/>
       <c r="S36"/>
       <c r="T36"/>
@@ -31789,10 +31788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36:AE36"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32259,7 +32256,7 @@
         <v>2</v>
       </c>
       <c r="AI11" s="45" t="s">
-        <v>227</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32363,7 +32360,7 @@
         <v>3</v>
       </c>
       <c r="AI12" s="45" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32467,7 +32464,7 @@
         <v>4</v>
       </c>
       <c r="AI13" s="45" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32571,7 +32568,7 @@
         <v>5</v>
       </c>
       <c r="AI14" s="45" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32675,7 +32672,7 @@
         <v>6</v>
       </c>
       <c r="AI15" s="45" t="s">
-        <v>264</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32779,7 +32776,7 @@
         <v>7</v>
       </c>
       <c r="AI16" s="45" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32883,7 +32880,7 @@
         <v>8</v>
       </c>
       <c r="AI17" s="45" t="s">
-        <v>266</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32987,7 +32984,7 @@
         <v>9</v>
       </c>
       <c r="AI18" s="45" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33091,7 +33088,7 @@
         <v>10</v>
       </c>
       <c r="AI19" s="45" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33195,7 +33192,7 @@
         <v>11</v>
       </c>
       <c r="AI20" s="45" t="s">
-        <v>269</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33299,7 +33296,7 @@
         <v>12</v>
       </c>
       <c r="AI21" s="45" t="s">
-        <v>270</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33403,7 +33400,7 @@
         <v>13</v>
       </c>
       <c r="AI22" s="45" t="s">
-        <v>271</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33507,7 +33504,7 @@
         <v>14</v>
       </c>
       <c r="AI23" s="45" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33611,7 +33608,7 @@
         <v>15</v>
       </c>
       <c r="AI24" s="45" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33715,7 +33712,7 @@
         <v>16</v>
       </c>
       <c r="AI25" s="45" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33819,7 +33816,7 @@
         <v>17</v>
       </c>
       <c r="AI26" s="45" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33923,7 +33920,7 @@
         <v>18</v>
       </c>
       <c r="AI27" s="45" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -34027,7 +34024,7 @@
         <v>19</v>
       </c>
       <c r="AI28" s="45" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -34130,9 +34127,6 @@
       <c r="AH29" s="46">
         <v>20</v>
       </c>
-      <c r="AI29" s="45" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="30" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
@@ -34234,9 +34228,6 @@
       <c r="AH30" s="46">
         <v>21</v>
       </c>
-      <c r="AI30" s="45" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="31" spans="1:35" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
@@ -35921,94 +35912,94 @@
         <v>78</v>
       </c>
       <c r="B48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA48" s="44">
         <v>0</v>
       </c>
       <c r="AB48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC48" s="44">
         <v>1</v>
       </c>
       <c r="AD48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE48" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF48" s="44">
         <v>0</v>
@@ -37195,94 +37186,94 @@
         <v>93</v>
       </c>
       <c r="B61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" s="41">
-        <v>1</v>
-      </c>
-      <c r="E61" s="44">
+        <v>0</v>
+      </c>
+      <c r="E61" s="41">
         <v>0</v>
       </c>
       <c r="F61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O61" s="41">
         <v>1</v>
       </c>
       <c r="P61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="41">
         <v>0</v>
@@ -37293,94 +37284,94 @@
         <v>94</v>
       </c>
       <c r="B62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" s="41">
-        <v>1</v>
-      </c>
-      <c r="E62" s="44">
+        <v>0</v>
+      </c>
+      <c r="E62" s="41">
         <v>0</v>
       </c>
       <c r="F62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O62" s="41">
         <v>1</v>
       </c>
       <c r="P62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE62" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF62" s="41">
         <v>0</v>
@@ -38371,96 +38362,96 @@
         <v>106</v>
       </c>
       <c r="B73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" s="44">
         <v>0</v>
       </c>
       <c r="F73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O73" s="44">
         <v>1</v>
       </c>
       <c r="P73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD73" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE73" s="44">
-        <v>1</v>
-      </c>
-      <c r="AF73" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="41">
         <v>0</v>
       </c>
     </row>
@@ -38469,96 +38460,96 @@
         <v>107</v>
       </c>
       <c r="B74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="44">
         <v>0</v>
       </c>
       <c r="F74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O74" s="44">
         <v>1</v>
       </c>
       <c r="P74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD74" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE74" s="44">
-        <v>1</v>
-      </c>
-      <c r="AF74" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="41">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to costs analysis
</commit_message>
<xml_diff>
--- a/MP Workbook LAUNCHPAD.xlsx
+++ b/MP Workbook LAUNCHPAD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="360" windowWidth="14430" windowHeight="11355" tabRatio="779" activeTab="3"/>
+    <workbookView xWindow="1995" yWindow="360" windowWidth="14430" windowHeight="11355" tabRatio="779"/>
   </bookViews>
   <sheets>
     <sheet name="MP_new" sheetId="4" r:id="rId1"/>
@@ -1806,11 +1806,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274920512"/>
-        <c:axId val="274921088"/>
+        <c:axId val="278512768"/>
+        <c:axId val="278513344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274920512"/>
+        <c:axId val="278512768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1840,12 +1840,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="274921088"/>
+        <c:crossAx val="278513344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="274921088"/>
+        <c:axId val="278513344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1875,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="274920512"/>
+        <c:crossAx val="278512768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2270,11 +2270,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="274922816"/>
-        <c:axId val="268550144"/>
+        <c:axId val="278515072"/>
+        <c:axId val="278515648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="274922816"/>
+        <c:axId val="278515072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2304,12 +2304,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268550144"/>
+        <c:crossAx val="278515648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="268550144"/>
+        <c:axId val="278515648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2344,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="274922816"/>
+        <c:crossAx val="278515072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2769,8 +2769,8 @@
   </sheetPr>
   <dimension ref="A1:CP200"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3312,7 +3312,7 @@
         <v>3</v>
       </c>
       <c r="Q11" s="87">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="R11" s="99"/>
       <c r="AI11" s="63"/>
@@ -32427,7 +32427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>

</xml_diff>